<commit_message>
Added two more plots (stat over time/level and hero comparison). Defined selected columns for hero comparison. Fixed some column name issues related to underscores. Added missing Attack Range. Implemented color blind mode. Basically almost done.
</commit_message>
<xml_diff>
--- a/Data/dictionary.xlsx
+++ b/Data/dictionary.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -115,7 +115,7 @@
     <t>HP Gain</t>
   </si>
   <si>
-    <t>HP_sb</t>
+    <t>HP_s_b</t>
   </si>
   <si>
     <t>Base HP Regeneration</t>
@@ -193,7 +193,7 @@
     <t>Base Mana</t>
   </si>
   <si>
-    <t>MP_sb</t>
+    <t>MP_s_b</t>
   </si>
   <si>
     <t>Base Mana Regeneration</t>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>Attack Rate</t>
+  </si>
+  <si>
+    <t>AtkRng</t>
+  </si>
+  <si>
+    <t>Attack Range</t>
   </si>
   <si>
     <t>DMG_avg_b</t>
@@ -351,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -363,6 +369,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,7 +729,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -824,7 +833,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -916,12 +925,12 @@
         <v>82</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>84</v>
@@ -981,6 +990,14 @@
       </c>
       <c r="B50" s="3" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed data import and stats sheet to allow multiple patches stored as individual sheets in the same .xlsx-file. Adjusted spaces in the hero comparison plot. Replaced the whole selectable and unselectable stat thing by having a character vector of unselectable stats in the input_constants script. Added Movement Speed calculation.
</commit_message>
<xml_diff>
--- a/Data/dictionary.xlsx
+++ b/Data/dictionary.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -308,6 +308,12 @@
   </si>
   <si>
     <t>Mana Regeneration</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Movement Speed</t>
   </si>
   <si>
     <t>AtkRngT</t>
@@ -1000,6 +1006,14 @@
         <v>100</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>